<commit_message>
Prepared for 3D printing. Moved from another repository
</commit_message>
<xml_diff>
--- a/docs/Servo calibration tables.xlsx
+++ b/docs/Servo calibration tables.xlsx
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F4" sqref="F4:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1066,7 @@
         <v>750</v>
       </c>
       <c r="F4" s="23">
-        <v>580</v>
+        <v>680</v>
       </c>
       <c r="G4" s="23">
         <v>610</v>
@@ -1093,7 +1093,7 @@
         <v>830</v>
       </c>
       <c r="F5" s="3">
-        <v>660</v>
+        <v>770</v>
       </c>
       <c r="G5" s="3">
         <v>680</v>
@@ -1120,7 +1120,7 @@
         <v>900</v>
       </c>
       <c r="F6" s="3">
-        <v>740</v>
+        <v>855</v>
       </c>
       <c r="G6" s="3">
         <v>750</v>
@@ -1147,7 +1147,7 @@
         <v>990</v>
       </c>
       <c r="F7" s="3">
-        <v>820</v>
+        <v>930</v>
       </c>
       <c r="G7" s="3">
         <v>830</v>
@@ -1174,7 +1174,7 @@
         <v>1070</v>
       </c>
       <c r="F8" s="3">
-        <v>915</v>
+        <v>1030</v>
       </c>
       <c r="G8" s="3">
         <v>910</v>
@@ -1201,7 +1201,7 @@
         <v>1160</v>
       </c>
       <c r="F9" s="3">
-        <v>990</v>
+        <v>1115</v>
       </c>
       <c r="G9" s="3">
         <v>990</v>
@@ -1228,7 +1228,7 @@
         <v>1240</v>
       </c>
       <c r="F10" s="3">
-        <v>1100</v>
+        <v>1210</v>
       </c>
       <c r="G10" s="3">
         <v>1070</v>
@@ -1255,7 +1255,7 @@
         <v>1330</v>
       </c>
       <c r="F11" s="3">
-        <v>1180</v>
+        <v>1300</v>
       </c>
       <c r="G11" s="3">
         <v>1160</v>
@@ -1282,7 +1282,7 @@
         <v>1410</v>
       </c>
       <c r="F12" s="3">
-        <v>1270</v>
+        <v>1400</v>
       </c>
       <c r="G12" s="3">
         <v>1240</v>
@@ -1309,7 +1309,7 @@
         <v>1500</v>
       </c>
       <c r="F13" s="20">
-        <v>1360</v>
+        <v>1500</v>
       </c>
       <c r="G13" s="20">
         <v>1320</v>
@@ -1336,7 +1336,7 @@
         <v>1600</v>
       </c>
       <c r="F14" s="3">
-        <v>1440</v>
+        <v>1610</v>
       </c>
       <c r="G14" s="3">
         <v>1400</v>
@@ -1363,7 +1363,7 @@
         <v>1690</v>
       </c>
       <c r="F15" s="3">
-        <v>1530</v>
+        <v>1700</v>
       </c>
       <c r="G15" s="3">
         <v>1480</v>
@@ -1390,7 +1390,7 @@
         <v>1770</v>
       </c>
       <c r="F16" s="3">
-        <v>1630</v>
+        <v>1790</v>
       </c>
       <c r="G16" s="3">
         <v>1560</v>
@@ -1417,7 +1417,7 @@
         <v>1860</v>
       </c>
       <c r="F17" s="3">
-        <v>1730</v>
+        <v>1890</v>
       </c>
       <c r="G17" s="3">
         <v>1640</v>
@@ -1444,7 +1444,7 @@
         <v>1950</v>
       </c>
       <c r="F18" s="3">
-        <v>1820</v>
+        <v>1970</v>
       </c>
       <c r="G18" s="3">
         <v>1720</v>
@@ -1471,7 +1471,7 @@
         <v>2030</v>
       </c>
       <c r="F19" s="3">
-        <v>1910</v>
+        <v>2075</v>
       </c>
       <c r="G19" s="3">
         <v>1800</v>
@@ -1498,7 +1498,7 @@
         <v>2120</v>
       </c>
       <c r="F20" s="3">
-        <v>2010</v>
+        <v>2180</v>
       </c>
       <c r="G20" s="3">
         <v>1900</v>
@@ -1525,7 +1525,7 @@
         <v>2210</v>
       </c>
       <c r="F21" s="3">
-        <v>2100</v>
+        <v>2280</v>
       </c>
       <c r="G21" s="3">
         <v>1970</v>
@@ -1552,7 +1552,7 @@
         <v>2300</v>
       </c>
       <c r="F22" s="3">
-        <v>2170</v>
+        <v>2380</v>
       </c>
       <c r="G22" s="3">
         <v>2070</v>
@@ -3210,11 +3210,11 @@
       </c>
       <c r="C3" s="7" t="str">
         <f>IF(ISBLANK(Tables!F4), DEC2HEX(65535), DEC2HEX(Tables!F4, 4))</f>
-        <v>0244</v>
+        <v>02A8</v>
       </c>
       <c r="D3" s="9" t="str">
         <f>MID(C3,1,2)&amp;" "&amp;MID(C3,3,2)&amp;" "</f>
-        <v xml:space="preserve">02 44 </v>
+        <v xml:space="preserve">02 A8 </v>
       </c>
       <c r="G3" s="52" t="s">
         <v>0</v>
@@ -3235,11 +3235,11 @@
       </c>
       <c r="C4" s="7" t="str">
         <f>IF(ISBLANK(Tables!F5), DEC2HEX(65535), DEC2HEX(Tables!F5, 4))</f>
-        <v>0294</v>
+        <v>0302</v>
       </c>
       <c r="D4" s="9" t="str">
         <f t="shared" ref="D4:D30" si="0">MID(C4,1,2)&amp;" "&amp;MID(C4,3,2)&amp;" "</f>
-        <v xml:space="preserve">02 94 </v>
+        <v xml:space="preserve">03 02 </v>
       </c>
       <c r="F4" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3)) + 0, 4)</f>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="G4" s="46" t="str">
         <f>F4&amp;":                           "&amp;D3&amp;D4&amp;" "&amp;D5&amp;D6</f>
-        <v xml:space="preserve">0348:                           02 44 02 94  02 E4 03 34 </v>
+        <v xml:space="preserve">0348:                           02 A8 03 02  03 57 03 A2 </v>
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="47"/>
@@ -3263,11 +3263,11 @@
       </c>
       <c r="C5" s="7" t="str">
         <f>IF(ISBLANK(Tables!F6), DEC2HEX(65535), DEC2HEX(Tables!F6, 4))</f>
-        <v>02E4</v>
+        <v>0357</v>
       </c>
       <c r="D5" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">02 E4 </v>
+        <v xml:space="preserve">03 57 </v>
       </c>
       <c r="F5" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+8, 4)</f>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="G5" s="46" t="str">
         <f>F5&amp;": "&amp;D7&amp;D8&amp;" "&amp;D9&amp;D10&amp;" "&amp;D11&amp;D12&amp;" "&amp;D13&amp;D14</f>
-        <v xml:space="preserve">0350: 03 93 03 DE  04 4C 04 9C  04 F6 05 50  05 A0 05 FA </v>
+        <v xml:space="preserve">0350: 04 06 04 5B  04 BA 05 14  05 78 05 DC  06 4A 06 A4 </v>
       </c>
       <c r="H5" s="47"/>
       <c r="I5" s="47"/>
@@ -3291,11 +3291,11 @@
       </c>
       <c r="C6" s="7" t="str">
         <f>IF(ISBLANK(Tables!F7), DEC2HEX(65535), DEC2HEX(Tables!F7, 4))</f>
-        <v>0334</v>
+        <v>03A2</v>
       </c>
       <c r="D6" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">03 34 </v>
+        <v xml:space="preserve">03 A2 </v>
       </c>
       <c r="F6" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+24, 4)</f>
@@ -3303,7 +3303,7 @@
       </c>
       <c r="G6" s="46" t="str">
         <f>F6&amp;": "&amp;D15&amp;D16&amp;" "&amp;D17&amp;D18&amp;" "&amp;D19&amp;D20&amp;" "&amp;D21&amp;D22</f>
-        <v xml:space="preserve">0360: 06 5E 06 C2  07 1C 07 76  07 DA 08 34  08 7A FF FF </v>
+        <v xml:space="preserve">0360: 06 FE 07 62  07 B2 08 1B  08 84 08 E8  09 4C FF FF </v>
       </c>
       <c r="H6" s="47"/>
       <c r="I6" s="47"/>
@@ -3319,11 +3319,11 @@
       </c>
       <c r="C7" s="7" t="str">
         <f>IF(ISBLANK(Tables!F8), DEC2HEX(65535), DEC2HEX(Tables!F8, 4))</f>
-        <v>0393</v>
+        <v>0406</v>
       </c>
       <c r="D7" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">03 93 </v>
+        <v xml:space="preserve">04 06 </v>
       </c>
       <c r="F7" s="13" t="str">
         <f>DEC2HEX( VALUE(HEX2DEC($I$3))+40, 4)</f>
@@ -3347,11 +3347,11 @@
       </c>
       <c r="C8" s="7" t="str">
         <f>IF(ISBLANK(Tables!F9), DEC2HEX(65535), DEC2HEX(Tables!F9, 4))</f>
-        <v>03DE</v>
+        <v>045B</v>
       </c>
       <c r="D8" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">03 DE </v>
+        <v xml:space="preserve">04 5B </v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -3361,11 +3361,11 @@
       </c>
       <c r="C9" s="7" t="str">
         <f>IF(ISBLANK(Tables!F10), DEC2HEX(65535), DEC2HEX(Tables!F10, 4))</f>
-        <v>044C</v>
+        <v>04BA</v>
       </c>
       <c r="D9" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">04 4C </v>
+        <v xml:space="preserve">04 BA </v>
       </c>
       <c r="F9" s="10"/>
     </row>
@@ -3375,11 +3375,11 @@
       </c>
       <c r="C10" s="7" t="str">
         <f>IF(ISBLANK(Tables!F11), DEC2HEX(65535), DEC2HEX(Tables!F11, 4))</f>
-        <v>049C</v>
+        <v>0514</v>
       </c>
       <c r="D10" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">04 9C </v>
+        <v xml:space="preserve">05 14 </v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -3389,11 +3389,11 @@
       </c>
       <c r="C11" s="7" t="str">
         <f>IF(ISBLANK(Tables!F12), DEC2HEX(65535), DEC2HEX(Tables!F12, 4))</f>
-        <v>04F6</v>
+        <v>0578</v>
       </c>
       <c r="D11" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">04 F6 </v>
+        <v xml:space="preserve">05 78 </v>
       </c>
       <c r="F11" s="10"/>
     </row>
@@ -3403,11 +3403,11 @@
       </c>
       <c r="C12" s="7" t="str">
         <f>IF(ISBLANK(Tables!F13), DEC2HEX(65535), DEC2HEX(Tables!F13, 4))</f>
-        <v>0550</v>
+        <v>05DC</v>
       </c>
       <c r="D12" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">05 50 </v>
+        <v xml:space="preserve">05 DC </v>
       </c>
       <c r="F12" s="10"/>
     </row>
@@ -3417,11 +3417,11 @@
       </c>
       <c r="C13" s="7" t="str">
         <f>IF(ISBLANK(Tables!F14), DEC2HEX(65535), DEC2HEX(Tables!F14, 4))</f>
-        <v>05A0</v>
+        <v>064A</v>
       </c>
       <c r="D13" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">05 A0 </v>
+        <v xml:space="preserve">06 4A </v>
       </c>
       <c r="F13" s="10"/>
     </row>
@@ -3431,11 +3431,11 @@
       </c>
       <c r="C14" s="7" t="str">
         <f>IF(ISBLANK(Tables!F15), DEC2HEX(65535), DEC2HEX(Tables!F15, 4))</f>
-        <v>05FA</v>
+        <v>06A4</v>
       </c>
       <c r="D14" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">05 FA </v>
+        <v xml:space="preserve">06 A4 </v>
       </c>
       <c r="F14" s="10"/>
     </row>
@@ -3445,11 +3445,11 @@
       </c>
       <c r="C15" s="7" t="str">
         <f>IF(ISBLANK(Tables!F16), DEC2HEX(65535), DEC2HEX(Tables!F16, 4))</f>
-        <v>065E</v>
+        <v>06FE</v>
       </c>
       <c r="D15" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">06 5E </v>
+        <v xml:space="preserve">06 FE </v>
       </c>
       <c r="F15" s="10"/>
     </row>
@@ -3459,11 +3459,11 @@
       </c>
       <c r="C16" s="7" t="str">
         <f>IF(ISBLANK(Tables!F17), DEC2HEX(65535), DEC2HEX(Tables!F17, 4))</f>
-        <v>06C2</v>
+        <v>0762</v>
       </c>
       <c r="D16" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">06 C2 </v>
+        <v xml:space="preserve">07 62 </v>
       </c>
       <c r="F16" s="10"/>
     </row>
@@ -3473,11 +3473,11 @@
       </c>
       <c r="C17" s="7" t="str">
         <f>IF(ISBLANK(Tables!F18), DEC2HEX(65535), DEC2HEX(Tables!F18, 4))</f>
-        <v>071C</v>
+        <v>07B2</v>
       </c>
       <c r="D17" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">07 1C </v>
+        <v xml:space="preserve">07 B2 </v>
       </c>
       <c r="F17" s="10"/>
     </row>
@@ -3487,11 +3487,11 @@
       </c>
       <c r="C18" s="7" t="str">
         <f>IF(ISBLANK(Tables!F19), DEC2HEX(65535), DEC2HEX(Tables!F19, 4))</f>
-        <v>0776</v>
+        <v>081B</v>
       </c>
       <c r="D18" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">07 76 </v>
+        <v xml:space="preserve">08 1B </v>
       </c>
       <c r="F18" s="10"/>
     </row>
@@ -3501,11 +3501,11 @@
       </c>
       <c r="C19" s="7" t="str">
         <f>IF(ISBLANK(Tables!F20), DEC2HEX(65535), DEC2HEX(Tables!F20, 4))</f>
-        <v>07DA</v>
+        <v>0884</v>
       </c>
       <c r="D19" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">07 DA </v>
+        <v xml:space="preserve">08 84 </v>
       </c>
       <c r="F19" s="10"/>
     </row>
@@ -3515,11 +3515,11 @@
       </c>
       <c r="C20" s="7" t="str">
         <f>IF(ISBLANK(Tables!F21), DEC2HEX(65535), DEC2HEX(Tables!F21, 4))</f>
-        <v>0834</v>
+        <v>08E8</v>
       </c>
       <c r="D20" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">08 34 </v>
+        <v xml:space="preserve">08 E8 </v>
       </c>
       <c r="F20" s="10"/>
     </row>
@@ -3529,11 +3529,11 @@
       </c>
       <c r="C21" s="7" t="str">
         <f>IF(ISBLANK(Tables!F22), DEC2HEX(65535), DEC2HEX(Tables!F22, 4))</f>
-        <v>087A</v>
+        <v>094C</v>
       </c>
       <c r="D21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">08 7A </v>
+        <v xml:space="preserve">09 4C </v>
       </c>
       <c r="F21" s="10"/>
     </row>

</xml_diff>